<commit_message>
Cambios Modulo Orden y Empresa
</commit_message>
<xml_diff>
--- a/reporteOrdenes.xlsx
+++ b/reporteOrdenes.xlsx
@@ -4,21 +4,21 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="75" windowWidth="17055" windowHeight="10830" activeTab="1"/>
+    <workbookView xWindow="32760" yWindow="32760" windowWidth="28800" windowHeight="12435" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Exportacion" sheetId="1" r:id="rId3"/>
     <sheet name="Evaluation Warning" sheetId="2" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="Exportacion">Exportacion!$A$1:$AM$20</definedName>
+    <definedName name="Exportacion">Exportacion!$A$1:$AM$27</definedName>
   </definedNames>
   <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="194">
   <si>
     <t>Número</t>
   </si>
@@ -137,19 +137,20 @@
     <t>Encendido Por Motor</t>
   </si>
   <si>
-    <t>I.M. MALDONADO</t>
-  </si>
-  <si>
-    <t>BIM176</t>
-  </si>
-  <si>
-    <t>Para asignar</t>
-  </si>
-  <si>
-    <t>I.M. MALDONADO TRANSPORTE</t>
-  </si>
-  <si>
-    <t>I.M.MALDONADO-MOTOS Y MAQUINARIA LIVIANA</t>
+    <t>MTOP - DIRECCION NAL. DE VIALIDAD</t>
+  </si>
+  <si>
+    <t>SOF9037</t>
+  </si>
+  <si>
+    <t>MTOP - DNVialidad - Conservacion</t>
+  </si>
+  <si>
+    <t>MTOP-DNVial - Conservacion - GAS OIL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(21/07/22 12:13 - Ricardo Cardozo): se instala fop_x000d_
+</t>
   </si>
   <si>
     <t>No</t>
@@ -158,203 +159,326 @@
     <t>Montevideo</t>
   </si>
   <si>
-    <t>Corralon</t>
+    <t>Taller</t>
   </si>
   <si>
     <t>0</t>
   </si>
   <si>
-    <t>MTOP - DIRECCION NAL. DE VIALIDAD</t>
+    <t>UTE</t>
+  </si>
+  <si>
+    <t>RF338</t>
+  </si>
+  <si>
+    <t>895980161834385401 (091385401)</t>
+  </si>
+  <si>
+    <t>TRA EST GRT CRM - CRT MONTEVIDEO</t>
+  </si>
+  <si>
+    <t>TRA EST GRT CRM - GAS OIL COMÚN 50S</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(20/07/22 13:22 - Nicolás Álvarez): se coloca dpl fop y bobina_x000d_
+</t>
+  </si>
+  <si>
+    <t>Sí</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jujuy 2627 </t>
+  </si>
+  <si>
+    <t>UDELAR - CURE</t>
+  </si>
+  <si>
+    <t>COF1183</t>
+  </si>
+  <si>
+    <t>895980161764054322 (091054322)</t>
+  </si>
+  <si>
+    <t>UDELAR - Centro Universitario Regional Este</t>
+  </si>
+  <si>
+    <t>UDELAR- C.Universitario Reg. Este Nafta Super</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(22/07/22 10:53 - Ricardo Cardozo): se instala fop y dpl_x000d_
+</t>
+  </si>
+  <si>
+    <t>LABANEL</t>
+  </si>
+  <si>
+    <t>UTU - CETP</t>
+  </si>
+  <si>
+    <t>SOF8967</t>
+  </si>
+  <si>
+    <t>UTU - Flota de Ruta</t>
+  </si>
+  <si>
+    <t>1906 - UTU - F.Ruta - Mdeo - SUPER 30-S</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(21/07/22 13:16 - Ricardo Cardozo): se instala fop_x000d_
+</t>
   </si>
   <si>
     <t>LAL7377</t>
   </si>
   <si>
-    <t>MTOP - DNVialidad - Conservacion</t>
+    <t>895980161834385459 (091385459)</t>
   </si>
   <si>
     <t>MTOP-DNVialidad-Conservación Super 95</t>
   </si>
   <si>
-    <t>Sí</t>
-  </si>
-  <si>
-    <t>Taller</t>
+    <t xml:space="preserve">(20/07/22 10:32 - Ricardo Cardozo): se instala fop y dpl_x000d_
+</t>
   </si>
   <si>
     <t>LAL7378</t>
   </si>
   <si>
+    <t>895980161263898672 (091898672)</t>
+  </si>
+  <si>
     <t>MTOP - DNVialidad - Construcciones</t>
   </si>
   <si>
     <t>MTOP-DNVial - Construcciones - SUPRA 95</t>
   </si>
   <si>
+    <t xml:space="preserve">(20/07/22 12:04 - Sergio Piñero): se instala dpl mas fop_x000d_
+</t>
+  </si>
+  <si>
     <t>LAL7379</t>
   </si>
   <si>
+    <t>895980101854097384 (091097384)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(20/07/22 14:52 - Sergio Piñero): se instala dpl mas fop_x000d_
+</t>
+  </si>
+  <si>
     <t>LAL9243</t>
   </si>
   <si>
+    <t>895980101854104644 (091104644)</t>
+  </si>
+  <si>
     <t>MTOP - DNVialidad - Regional 6</t>
   </si>
   <si>
     <t>MTOP-DNVialidad-Regional 6 - Super 95</t>
   </si>
   <si>
+    <t xml:space="preserve">(21/07/22 16:18 - Nicolás Álvarez): se instala dpl fop y bobina_x000d_
+(21/07/22 16:23 - Nicolás Álvarez): se cambia dpl_x000d_
+(21/07/22 16:44 - Nicolás Álvarez): se cambia dpl_x000d_
+(21/07/22 16:47 - Nicolás Álvarez): se cambia dpl_x000d_
+(21/07/22 16:56 - Nicolás Álvarez): se cambia dpl_x000d_
+(21/07/22 17:02 - Nicolás Álvarez): se cambia dpl_x000d_
+</t>
+  </si>
+  <si>
     <t>LAL9244</t>
   </si>
   <si>
+    <t>895980161744523205 (091523205)</t>
+  </si>
+  <si>
     <t>MTOP-DNVial - Regional 6 - GAS OIL</t>
   </si>
   <si>
+    <t xml:space="preserve">(20/07/22 15:42 - Nicolás Álvarez): se coloca dpl fop y bobina_x000d_
+(20/07/22 16:05 - Nicolás Álvarez): se coloca dpl fop y bobina_x000d_
+</t>
+  </si>
+  <si>
     <t>SOF8981</t>
   </si>
   <si>
-    <t>MTOP-DNVial - Conservacion - GAS OIL</t>
+    <t>895980161664565856 (091565856)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(21/07/22 11:52 - Luis Risotto): se instala dpl ,fo y bobina_x000d_
+</t>
+  </si>
+  <si>
+    <t>MINISTERIO DE TURISMO</t>
+  </si>
+  <si>
+    <t>SOF9083</t>
+  </si>
+  <si>
+    <t>895980161754881218 (091881218)</t>
+  </si>
+  <si>
+    <t>SECRETARIA</t>
+  </si>
+  <si>
+    <t>M.TUR. Flota - Supra 95</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(20/07/22 12:03 - Nicolás Álvarez): se coloca dpl fop y bobina_x000d_
+(20/07/22 12:08 - Nicolás Álvarez): se coloca dpl fop y bobina_x000d_
+(20/07/22 12:15 - Nicolás Álvarez): se coloca dpl fop y bobina_x000d_
+</t>
+  </si>
+  <si>
+    <t>INAU</t>
+  </si>
+  <si>
+    <t>BEB3777</t>
+  </si>
+  <si>
+    <t>895980161754818584 (091818584)</t>
+  </si>
+  <si>
+    <t>SERVICIOS GENERALES</t>
+  </si>
+  <si>
+    <t>INAU Locomocion y Transporte Nafta 95</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(20/07/22 14:53 - Ricardo Cardozo): se instala fop y dpl_x000d_
+</t>
+  </si>
+  <si>
+    <t>OSE</t>
+  </si>
+  <si>
+    <t>SAL9489</t>
+  </si>
+  <si>
+    <t>895980101854097352 (091097352)</t>
+  </si>
+  <si>
+    <t>GCIA REGION LITORAL SUR - COLONIA</t>
+  </si>
+  <si>
+    <t>CARMELO - TECNICA - GAS OIL 50-S</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(21/07/22 15:14 - Luis Risotto): se coloca dpl bobina y fop_x000d_
+(21/07/22 15:35 - Luis Risotto): se cambia dpl_x000d_
+</t>
+  </si>
+  <si>
+    <t>I.M. FLORIDA</t>
+  </si>
+  <si>
+    <t>OIM1027</t>
+  </si>
+  <si>
+    <t>895980101854097426 (091097426)</t>
+  </si>
+  <si>
+    <t>PASEOS PUBLICOS</t>
+  </si>
+  <si>
+    <t>I.M.FLORIDA - PASEOS PUBLICOS - G. OIL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(21/07/22 09:56 - Sergio Piñero): se instala dpl mas fop_x000d_
+</t>
+  </si>
+  <si>
+    <t>Florida</t>
+  </si>
+  <si>
+    <t>Corralon Municipal</t>
+  </si>
+  <si>
+    <t>Zona 4</t>
+  </si>
+  <si>
+    <t>OID0001</t>
+  </si>
+  <si>
+    <t>DEPTO. DE ADMINISTRACION</t>
+  </si>
+  <si>
+    <t>1202 Depto de Admin Supra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(21/07/22 09:05 - Sergio Piñero): se instala solo fop_x000d_
+</t>
+  </si>
+  <si>
+    <t>Corralon municipal</t>
+  </si>
+  <si>
+    <t>MAH7500</t>
+  </si>
+  <si>
+    <t>895980161834465415 (091465415)</t>
+  </si>
+  <si>
+    <t>MTOP - DNVialidad - Apoyo</t>
+  </si>
+  <si>
+    <t>MTOP-DNVial - Apoyo - GAS OIL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(20/07/22 09:39 - Sergio Piñero): se instala fop mas dpl_x000d_
+</t>
+  </si>
+  <si>
+    <t>A.S.S.E.</t>
+  </si>
+  <si>
+    <t>MOF1566</t>
+  </si>
+  <si>
+    <t>895980101854097393 (091097393)</t>
+  </si>
+  <si>
+    <t>ASSE Bella Union</t>
+  </si>
+  <si>
+    <t>ASSE Bella Union Nafta 95</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(19/07/22 13:10 - Carina Sasía): Vehiculo desinstalado por error, se debe dejar el mismo gps._x000d_
+(22/07/22 15:00 - Nicolás Álvarez): se coloca dpl fop y bobina_x000d_
+(22/07/22 15:12 - Nicolás Álvarez): se cambia dpl_x000d_
+</t>
   </si>
   <si>
     <t>I.M. CANELONES</t>
   </si>
   <si>
-    <t>AIC2117</t>
-  </si>
-  <si>
-    <t>OBRAS</t>
-  </si>
-  <si>
-    <t>1214 OBRAS SUPER 95</t>
-  </si>
-  <si>
-    <t>CONSEJO DE EDUCACION PRIMARIA</t>
-  </si>
-  <si>
-    <t>SOF9079</t>
-  </si>
-  <si>
-    <t>3 - DIVISION EDUCACION - CEIP</t>
-  </si>
-  <si>
-    <t>208 CEP - Div .Ed. MDEO - Gas Oil</t>
-  </si>
-  <si>
-    <t>MINISTERIO DE TURISMO</t>
-  </si>
-  <si>
-    <t>SOF9083</t>
-  </si>
-  <si>
-    <t>SECRETARIA</t>
-  </si>
-  <si>
-    <t>M.TUR. Flota - Supra 95</t>
-  </si>
-  <si>
-    <t>INAU</t>
-  </si>
-  <si>
-    <t>BEB3777</t>
-  </si>
-  <si>
-    <t>SERVICIOS GENERALES</t>
-  </si>
-  <si>
-    <t>INAU Locomocion y Transporte Nafta 95</t>
-  </si>
-  <si>
-    <t>OSE</t>
-  </si>
-  <si>
-    <t>SAL9489</t>
-  </si>
-  <si>
-    <t>GCIA REGION LITORAL SUR - COLONIA</t>
-  </si>
-  <si>
-    <t>CARMELO - TECNICA - GAS OIL 50-S</t>
-  </si>
-  <si>
-    <t>I.M. FLORIDA</t>
-  </si>
-  <si>
-    <t>OIM1027</t>
-  </si>
-  <si>
-    <t>PASEOS PUBLICOS</t>
-  </si>
-  <si>
-    <t>I.M.FLORIDA - PASEOS PUBLICOS - G. OIL</t>
-  </si>
-  <si>
-    <t>Florida</t>
-  </si>
-  <si>
-    <t>Corralon Municipal</t>
-  </si>
-  <si>
-    <t>Zona 4</t>
-  </si>
-  <si>
-    <t>MOTO22</t>
-  </si>
-  <si>
-    <t>DIRECCION GRAL. DE OBRAS</t>
-  </si>
-  <si>
-    <t>471 I.M.FLORIDA - D.G.DE OBRAS - G. OIL</t>
-  </si>
-  <si>
-    <t>OID0001</t>
-  </si>
-  <si>
-    <t>DEPTO. DE ADMINISTRACION</t>
-  </si>
-  <si>
-    <t>1202 Depto de Admin Supra</t>
-  </si>
-  <si>
-    <t>Corralon municipal</t>
-  </si>
-  <si>
-    <t>MAH7500</t>
-  </si>
-  <si>
-    <t>MTOP - DNVialidad - Apoyo</t>
-  </si>
-  <si>
-    <t>MTOP-DNVial - Apoyo - GAS OIL</t>
-  </si>
-  <si>
-    <t>A.S.S.E.</t>
-  </si>
-  <si>
-    <t>MOF1566</t>
-  </si>
-  <si>
-    <t>ASSE Bella Union</t>
-  </si>
-  <si>
-    <t>ASSE Bella Union Nafta 95</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(19/07/22 13:10 - Carina Sasía): Vehiculo desinstalado por error, se debe dejar el mismo gps._x000d_
+    <t>AIC2173</t>
+  </si>
+  <si>
+    <t>895980161744473404 (091473404)</t>
+  </si>
+  <si>
+    <t>LOCOMOCION</t>
+  </si>
+  <si>
+    <t>495- I.M.CANEL.NUEVA FLOTA - G.O.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(20/07/22 15:07 - Luis Risotto): se instala dpl bobina y fop_x000d_
 </t>
   </si>
   <si>
-    <t>AIC2173</t>
-  </si>
-  <si>
-    <t>LOCOMOCION</t>
-  </si>
-  <si>
-    <t>495- I.M.CANEL.NUEVA FLOTA - G.O.</t>
-  </si>
-  <si>
     <t>I.M. MONTEVIDEO</t>
   </si>
   <si>
     <t>SIM2995</t>
+  </si>
+  <si>
+    <t>895980161754746218 (091746218)</t>
   </si>
   <si>
     <t>LIMPIEZA</t>
@@ -365,10 +489,153 @@
   <si>
     <t xml:space="preserve">(19/07/22 16:17 - Carina Sasía): Walter Piedad  095043349_x000d_
 Disposicion final, Felipe cardozo 3220_x000d_
+(22/07/22 09:50 - Sergio Piñero): se instala dpl mas fop_x000d_
 </t>
   </si>
   <si>
     <t>Felipe Cardozo 3220</t>
+  </si>
+  <si>
+    <t>OID1248</t>
+  </si>
+  <si>
+    <t>895980161754828361 (091828361)</t>
+  </si>
+  <si>
+    <t>DEPTO. DE HIGIENE</t>
+  </si>
+  <si>
+    <t>473 I.M.FLORIDA - DEPTO DE HIGIENE - G. OIL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(21/07/22 13:08 - Sergio Piñero): se coloco dpl mas fop_x000d_
+</t>
+  </si>
+  <si>
+    <t>IM Florida</t>
+  </si>
+  <si>
+    <t>MINISTERIO DEL INTERIOR</t>
+  </si>
+  <si>
+    <t>S04714</t>
+  </si>
+  <si>
+    <t>895980161834080686 (091080686)</t>
+  </si>
+  <si>
+    <t>MI -06-JPCanelones</t>
+  </si>
+  <si>
+    <t>MI - JPCANELONES Gasoil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(22/07/22 11:51 - Nicolás Álvarez): se coloca dpl fop y bobina_x000d_
+</t>
+  </si>
+  <si>
+    <t>SIM1204</t>
+  </si>
+  <si>
+    <t>895980101964879222 (091879222)</t>
+  </si>
+  <si>
+    <t>GESTIÓN HUMANA Y RECURSOS MATERIALES</t>
+  </si>
+  <si>
+    <t>GERENCIA DE MANTENIMIENTO DE FLOTA - GAS OIL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(20/07/22 14:05 - Carina Sasía): Pablo Vidal 099833403_x000d_
+(25/07/22 13:55 - Sergio Piñero): se coloca dpl y fop_x000d_
+</t>
+  </si>
+  <si>
+    <t>Coronel Raiz 1058</t>
+  </si>
+  <si>
+    <t>AGENCIA NACIONAL DE VIVIENDA</t>
+  </si>
+  <si>
+    <t>LAL6838</t>
+  </si>
+  <si>
+    <t>895980101854094517 (091094517)</t>
+  </si>
+  <si>
+    <t>751 SERVICIOS GENERALES</t>
+  </si>
+  <si>
+    <t>1596 - AG.NAL.VIVIENDA-SCIOS.GENERALES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(22/07/22 17:16 - Ricardo Cardozo): SE INSTALA FOP Y DPL_x000d_
+</t>
+  </si>
+  <si>
+    <t>MIEM - U.E 011 - A.R.N.R</t>
+  </si>
+  <si>
+    <t>SOF8593</t>
+  </si>
+  <si>
+    <t>895980101844671144 (091671144)</t>
+  </si>
+  <si>
+    <t>MIEM - A.R.N.R - AUT.REG.NAL.EN RADIOPROTECCION</t>
+  </si>
+  <si>
+    <t>MIEM - ARNR - SUPER 95 30S</t>
+  </si>
+  <si>
+    <t>UDELAR - FAC. DE AGRONOMÍA</t>
+  </si>
+  <si>
+    <t>SOF9875</t>
+  </si>
+  <si>
+    <t>895980161754746097 (091746097)</t>
+  </si>
+  <si>
+    <t>SCIOS. MONTEVIDEO</t>
+  </si>
+  <si>
+    <t>FORESTAL - SUPER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(25/07/22 13:24 - Ricardo Cardozo): se instala fop y dpl_x000d_
+</t>
+  </si>
+  <si>
+    <t>I.M. TACUAREMBO</t>
+  </si>
+  <si>
+    <t>RID1015S</t>
+  </si>
+  <si>
+    <t>895980161764054093 (091054093)</t>
+  </si>
+  <si>
+    <t>JUNTA PASO DE LOS TOROS</t>
+  </si>
+  <si>
+    <t>827 -J.P.TOROS-D.GRAL-SERV-G.OIL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(22/07/22 12:18 - Martin Ferrari): Se instala Fop y GPS_x000d_
+</t>
+  </si>
+  <si>
+    <t>Tacuarembó</t>
+  </si>
+  <si>
+    <t>Paso de los toros</t>
+  </si>
+  <si>
+    <t>Zona 1</t>
+  </si>
+  <si>
+    <t>Para asignar</t>
   </si>
   <si>
     <t>Evaluation Only. Created with Aspose.Cells for .NET.Copyright 2003 - 2022 Aspose Pty Ltd.</t>
@@ -378,54 +645,179 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="8">
-    <numFmt numFmtId="5" formatCode="&quot;$&quot;\ #,##0;\-&quot;$&quot;\ #,##0"/>
-    <numFmt numFmtId="6" formatCode="&quot;$&quot;\ #,##0;[Red]\-&quot;$&quot;\ #,##0"/>
-    <numFmt numFmtId="7" formatCode="&quot;$&quot;\ #,##0.00;\-&quot;$&quot;\ #,##0.00"/>
-    <numFmt numFmtId="8" formatCode="&quot;$&quot;\ #,##0.00;[Red]\-&quot;$&quot;\ #,##0.00"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;$&quot;\ * #,##0_-;\-&quot;$&quot;\ * #,##0_-;_-&quot;$&quot;\ * &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+  <numFmts count="23">
+    <numFmt numFmtId="5" formatCode="&quot;$&quot;#,##0_);\(&quot;$&quot;#,##0\)"/>
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+    <numFmt numFmtId="7" formatCode="&quot;$&quot;#,##0.00_);\(&quot;$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="&quot;$U&quot;\ #,##0_);\(&quot;$U&quot;\ #,##0\)"/>
+    <numFmt numFmtId="165" formatCode="&quot;$U&quot;\ #,##0_);[Red]\(&quot;$U&quot;\ #,##0\)"/>
+    <numFmt numFmtId="166" formatCode="&quot;$U&quot;\ #,##0.00_);\(&quot;$U&quot;\ #,##0.00\)"/>
+    <numFmt numFmtId="167" formatCode="&quot;$U&quot;\ #,##0.00_);[Red]\(&quot;$U&quot;\ #,##0.00\)"/>
+    <numFmt numFmtId="168" formatCode="_(&quot;$U&quot;\ * #,##0_);_(&quot;$U&quot;\ * \(#,##0\);_(&quot;$U&quot;\ * &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="169" formatCode="_(&quot;$U&quot;\ * #,##0.00_);_(&quot;$U&quot;\ * \(#,##0.00\);_(&quot;$U&quot;\ * &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="170" formatCode="&quot;$&quot;\ #,##0;\-&quot;$&quot;\ #,##0"/>
+    <numFmt numFmtId="171" formatCode="&quot;$&quot;\ #,##0;[Red]\-&quot;$&quot;\ #,##0"/>
+    <numFmt numFmtId="172" formatCode="&quot;$&quot;\ #,##0.00;\-&quot;$&quot;\ #,##0.00"/>
+    <numFmt numFmtId="173" formatCode="&quot;$&quot;\ #,##0.00;[Red]\-&quot;$&quot;\ #,##0.00"/>
+    <numFmt numFmtId="174" formatCode="_-&quot;$&quot;\ * #,##0_-;\-&quot;$&quot;\ * #,##0_-;_-&quot;$&quot;\ * &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="175" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="mmm\-yyyy"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="41">
     <font>
       <sz val="10"/>
       <name val="MS Sans Serif"/>
-      <family val="32"/>
+      <family val="0"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <name val="MS Sans Serif"/>
-      <family val="32"/>
+      <family val="0"/>
     </font>
     <font>
       <i/>
       <sz val="10"/>
       <name val="MS Sans Serif"/>
-      <family val="32"/>
+      <family val="0"/>
     </font>
     <font>
       <b/>
       <i/>
       <sz val="10"/>
       <name val="MS Sans Serif"/>
-      <family val="32"/>
+      <family val="0"/>
     </font>
     <font>
       <u val="single"/>
       <sz val="10"/>
       <color indexed="12"/>
       <name val="MS Sans Serif"/>
-      <family val="32"/>
+      <family val="0"/>
     </font>
     <font>
       <u val="single"/>
       <sz val="10"/>
       <color indexed="14"/>
       <name val="MS Sans Serif"/>
-      <family val="32"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="17"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="52"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="52"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color indexed="54"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="54"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="62"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="20"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="60"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="63"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color indexed="23"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color indexed="54"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color indexed="54"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -433,18 +825,331 @@
       <sz val="18"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
-      <family val="32"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.7999799847602844"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.7999799847602844"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.7999799847602844"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.7999799847602844"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.7999799847602844"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.7999799847602844"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.5999900102615356"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.5999900102615356"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.5999900102615356"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.5999900102615356"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.5999900102615356"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.5999900102615356"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39998000860214233"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39998000860214233"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39998000860214233"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39998000860214233"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39998000860214233"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39998000860214233"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -452,8 +1157,134 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color indexed="0"/>
+      </left>
+      <right>
+        <color indexed="0"/>
+      </right>
+      <top>
+        <color indexed="0"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color indexed="0"/>
+      </left>
+      <right>
+        <color indexed="0"/>
+      </right>
+      <top>
+        <color indexed="0"/>
+      </top>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color indexed="0"/>
+      </left>
+      <right>
+        <color indexed="0"/>
+      </right>
+      <top>
+        <color indexed="0"/>
+      </top>
+      <bottom style="thick">
+        <color theme="4" tint="0.49998000264167786"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color indexed="0"/>
+      </left>
+      <right>
+        <color indexed="0"/>
+      </right>
+      <top>
+        <color indexed="0"/>
+      </top>
+      <bottom style="medium">
+        <color theme="4" tint="0.39998000860214233"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color indexed="0"/>
+      </left>
+      <right>
+        <color indexed="0"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+    </border>
   </borders>
-  <cellStyleXfs count="22">
+  <cellStyleXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment/>
       <protection/>
@@ -472,19 +1303,57 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="40" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="40" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="40" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="40" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="40" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="40" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="40" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="40" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="40" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="40" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="40" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="40" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="34" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="34" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="34" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="34" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="34" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="34" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="39" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="21" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="22" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="34" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="34" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="34" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="34" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="34" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="34" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="33" fillId="29" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="175" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="31" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="32" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="30" fillId="21" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" quotePrefix="1">
       <alignment/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" quotePrefix="1">
@@ -493,21 +1362,63 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment/>
       <protection/>
     </xf>
   </cellXfs>
-  <cellStyles count="8">
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Followed Hyperlink" xfId="19" builtinId="9"/>
-    <cellStyle name="Hyperlink" xfId="20" builtinId="8"/>
-    <cellStyle name="Percent" xfId="21" builtinId="5"/>
+    <cellStyle name="20% - Énfasis1" xfId="15"/>
+    <cellStyle name="20% - Énfasis2" xfId="16"/>
+    <cellStyle name="20% - Énfasis3" xfId="17"/>
+    <cellStyle name="20% - Énfasis4" xfId="18"/>
+    <cellStyle name="20% - Énfasis5" xfId="19"/>
+    <cellStyle name="20% - Énfasis6" xfId="20"/>
+    <cellStyle name="40% - Énfasis1" xfId="21"/>
+    <cellStyle name="40% - Énfasis2" xfId="22"/>
+    <cellStyle name="40% - Énfasis3" xfId="23"/>
+    <cellStyle name="40% - Énfasis4" xfId="24"/>
+    <cellStyle name="40% - Énfasis5" xfId="25"/>
+    <cellStyle name="40% - Énfasis6" xfId="26"/>
+    <cellStyle name="60% - Énfasis1" xfId="27"/>
+    <cellStyle name="60% - Énfasis2" xfId="28"/>
+    <cellStyle name="60% - Énfasis3" xfId="29"/>
+    <cellStyle name="60% - Énfasis4" xfId="30"/>
+    <cellStyle name="60% - Énfasis5" xfId="31"/>
+    <cellStyle name="60% - Énfasis6" xfId="32"/>
+    <cellStyle name="Bueno" xfId="33"/>
+    <cellStyle name="Cálculo" xfId="34"/>
+    <cellStyle name="Celda de comprobación" xfId="35"/>
+    <cellStyle name="Celda vinculada" xfId="36"/>
+    <cellStyle name="Encabezado 1" xfId="37"/>
+    <cellStyle name="Encabezado 4" xfId="38"/>
+    <cellStyle name="Énfasis1" xfId="39"/>
+    <cellStyle name="Énfasis2" xfId="40"/>
+    <cellStyle name="Énfasis3" xfId="41"/>
+    <cellStyle name="Énfasis4" xfId="42"/>
+    <cellStyle name="Énfasis5" xfId="43"/>
+    <cellStyle name="Énfasis6" xfId="44"/>
+    <cellStyle name="Entrada" xfId="45"/>
+    <cellStyle name="Hyperlink" xfId="46" builtinId="8"/>
+    <cellStyle name="Followed Hyperlink" xfId="47" builtinId="9"/>
+    <cellStyle name="Incorrecto" xfId="48"/>
+    <cellStyle name="Comma" xfId="49" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="50" builtinId="6"/>
+    <cellStyle name="Currency" xfId="51" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="52" builtinId="7"/>
+    <cellStyle name="Neutral" xfId="53"/>
+    <cellStyle name="Notas" xfId="54"/>
+    <cellStyle name="Percent" xfId="55" builtinId="5"/>
+    <cellStyle name="Salida" xfId="56"/>
+    <cellStyle name="Texto de advertencia" xfId="57"/>
+    <cellStyle name="Texto explicativo" xfId="58"/>
+    <cellStyle name="Título" xfId="59"/>
+    <cellStyle name="Título 2" xfId="60"/>
+    <cellStyle name="Título 3" xfId="61"/>
+    <cellStyle name="Total" xfId="62"/>
   </cellStyles>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -588,7 +1499,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -604,7 +1515,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -616,7 +1527,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -633,9 +1544,9 @@
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -663,31 +1574,14 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -715,23 +1609,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -874,23 +1751,30 @@
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9ae4fdda-f3b9-4ac1-a86a-f0d1f95a59db}">
-  <dimension ref="A1:AM20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{c4e39d86-41f2-4ed1-a7aa-1d4461e27776}">
+  <dimension ref="A1:AM31"/>
   <sheetViews>
     <sheetView workbookViewId="0" topLeftCell="A1">
-      <selection pane="topLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="topLeft" activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="9.143973214285714" defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="5" width="9.142857142857142" customWidth="1"/>
+    <col min="6" max="6" width="12.285714285714286" customWidth="1"/>
+    <col min="7" max="7" width="11.142857142857142" customWidth="1"/>
+    <col min="8" max="8" width="12.857142857142858" customWidth="1"/>
+    <col min="9" max="20" width="9.142857142857142" customWidth="1"/>
+    <col min="21" max="21" width="40.857142857142854" customWidth="1"/>
+    <col min="22" max="23" width="9.142857142857142" customWidth="1"/>
+    <col min="24" max="24" width="34.714285714285715" customWidth="1"/>
+    <col min="25" max="25" width="15.285714285714286" customWidth="1"/>
+    <col min="26" max="16384" width="9.142857142857142"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:39" ht="12.75">
       <c r="A1" s="1" t="s">
@@ -1013,7 +1897,7 @@
     </row>
     <row r="2" spans="1:39" ht="12.75">
       <c r="A2" s="1">
-        <v>19448</v>
+        <v>19238</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>39</v>
@@ -1025,20 +1909,31 @@
         <v>40</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="F2" s="2">
+        <v>44767.490069444444</v>
+      </c>
+      <c r="G2" s="2">
+        <v>44779.490069444444</v>
+      </c>
+      <c r="H2" s="2"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="2"/>
+      <c r="T2" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F2" s="3">
-        <v>44754.490057870367</v>
-      </c>
-      <c r="G2" s="3">
-        <v>44757.490057870367</v>
-      </c>
-      <c r="T2" s="1" t="s">
+      <c r="U2" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="U2" s="1" t="s">
+      <c r="V2" s="1"/>
+      <c r="W2" s="1"/>
+      <c r="X2" s="1" t="s">
         <v>43</v>
       </c>
+      <c r="Y2" s="1"/>
       <c r="Z2" s="1" t="s">
         <v>44</v>
       </c>
@@ -1057,6 +1952,7 @@
       <c r="AE2" s="1" t="s">
         <v>46</v>
       </c>
+      <c r="AG2" s="1"/>
       <c r="AH2" s="1" t="s">
         <v>47</v>
       </c>
@@ -1078,7 +1974,7 @@
     </row>
     <row r="3" spans="1:39" ht="12.75">
       <c r="A3" s="1">
-        <v>19451</v>
+        <v>19327</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>48</v>
@@ -1090,22 +1986,37 @@
         <v>49</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F3" s="3">
-        <v>44754.512662037036</v>
-      </c>
-      <c r="G3" s="3">
-        <v>44779.512662037036</v>
+        <v>192</v>
+      </c>
+      <c r="F3" s="2">
+        <v>44767.490069444444</v>
+      </c>
+      <c r="G3" s="2">
+        <v>44750.386782407404</v>
+      </c>
+      <c r="H3" s="2"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="S3" s="1" t="s">
+        <v>50</v>
       </c>
       <c r="T3" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="U3" s="1" t="s">
-        <v>51</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="V3" s="1"/>
+      <c r="W3" s="1"/>
+      <c r="X3" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y3" s="1"/>
       <c r="Z3" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="AA3" s="1" t="s">
         <v>44</v>
@@ -1120,8 +2031,9 @@
         <v>45</v>
       </c>
       <c r="AE3" s="1" t="s">
-        <v>53</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="AG3" s="1"/>
       <c r="AH3" s="1" t="s">
         <v>47</v>
       </c>
@@ -1143,35 +2055,51 @@
     </row>
     <row r="4" spans="1:39" ht="12.75">
       <c r="A4" s="1">
-        <v>19452</v>
+        <v>19409</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="F4" s="2">
+        <v>44767.490069444444</v>
+      </c>
+      <c r="G4" s="2">
+        <v>44757.720949074072</v>
+      </c>
+      <c r="H4" s="2"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="S4" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="U4" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="V4" s="1"/>
+      <c r="W4" s="1"/>
+      <c r="X4" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="Y4" s="1"/>
+      <c r="Z4" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F4" s="3">
-        <v>44754.514386574076</v>
-      </c>
-      <c r="G4" s="3">
-        <v>44779.514386574076</v>
-      </c>
-      <c r="T4" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="U4" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="Z4" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="AA4" s="1" t="s">
         <v>44</v>
       </c>
@@ -1182,11 +2110,9 @@
         <v>44</v>
       </c>
       <c r="AD4" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="AE4" s="1" t="s">
-        <v>53</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="AG4" s="1"/>
       <c r="AH4" s="1" t="s">
         <v>47</v>
       </c>
@@ -1208,34 +2134,45 @@
     </row>
     <row r="5" spans="1:39" ht="12.75">
       <c r="A5" s="1">
-        <v>19453</v>
+        <v>19424</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F5" s="3">
-        <v>44754.515868055554</v>
-      </c>
-      <c r="G5" s="3">
-        <v>44779.515868055554</v>
-      </c>
+        <v>192</v>
+      </c>
+      <c r="F5" s="2">
+        <v>44767.490069444444</v>
+      </c>
+      <c r="G5" s="2">
+        <v>44764.618125000001</v>
+      </c>
+      <c r="H5" s="2"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="2"/>
       <c r="T5" s="1" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="U5" s="1" t="s">
-        <v>56</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="V5" s="1"/>
+      <c r="W5" s="1"/>
+      <c r="X5" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="Y5" s="1"/>
       <c r="Z5" s="1" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="AA5" s="1" t="s">
         <v>44</v>
@@ -1247,11 +2184,9 @@
         <v>44</v>
       </c>
       <c r="AD5" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="AE5" s="1" t="s">
-        <v>53</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="AG5" s="1"/>
       <c r="AH5" s="1" t="s">
         <v>47</v>
       </c>
@@ -1273,34 +2208,50 @@
     </row>
     <row r="6" spans="1:39" ht="12.75">
       <c r="A6" s="1">
-        <v>19454</v>
+        <v>19451</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="E6" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="F6" s="2">
+        <v>44767.490069444444</v>
+      </c>
+      <c r="G6" s="2">
+        <v>44779.512662037036</v>
+      </c>
+      <c r="H6" s="2"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="S6" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="T6" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F6" s="3">
-        <v>44754.517500000002</v>
-      </c>
-      <c r="G6" s="3">
-        <v>44779.517500000002</v>
-      </c>
-      <c r="T6" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="U6" s="1" t="s">
-        <v>60</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="V6" s="1"/>
+      <c r="W6" s="1"/>
+      <c r="X6" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="Y6" s="1"/>
       <c r="Z6" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="AA6" s="1" t="s">
         <v>44</v>
@@ -1315,8 +2266,9 @@
         <v>45</v>
       </c>
       <c r="AE6" s="1" t="s">
-        <v>53</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="AG6" s="1"/>
       <c r="AH6" s="1" t="s">
         <v>47</v>
       </c>
@@ -1338,34 +2290,49 @@
     </row>
     <row r="7" spans="1:39" ht="12.75">
       <c r="A7" s="1">
-        <v>19455</v>
+        <v>19452</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>61</v>
+        <v>72</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>61</v>
+        <v>72</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F7" s="3">
-        <v>44754.523275462961</v>
-      </c>
-      <c r="G7" s="3">
-        <v>44779.523275462961</v>
+        <v>192</v>
+      </c>
+      <c r="F7" s="2">
+        <v>44767.490069444444</v>
+      </c>
+      <c r="G7" s="2">
+        <v>44779.514386574076</v>
+      </c>
+      <c r="H7" s="2"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="S7" s="1" t="s">
+        <v>73</v>
       </c>
       <c r="T7" s="1" t="s">
-        <v>59</v>
+        <v>74</v>
       </c>
       <c r="U7" s="1" t="s">
-        <v>62</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="V7" s="1"/>
+      <c r="W7" s="1"/>
+      <c r="X7" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="Y7" s="1"/>
       <c r="Z7" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="AA7" s="1" t="s">
         <v>44</v>
@@ -1380,8 +2347,9 @@
         <v>45</v>
       </c>
       <c r="AE7" s="1" t="s">
-        <v>53</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="AG7" s="1"/>
       <c r="AH7" s="1" t="s">
         <v>47</v>
       </c>
@@ -1403,34 +2371,49 @@
     </row>
     <row r="8" spans="1:39" ht="12.75">
       <c r="A8" s="1">
-        <v>19456</v>
+        <v>19453</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>63</v>
+        <v>77</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>63</v>
+        <v>77</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F8" s="3">
-        <v>44754.530069444445</v>
-      </c>
-      <c r="G8" s="3">
-        <v>44779.530069444445</v>
+        <v>192</v>
+      </c>
+      <c r="F8" s="2">
+        <v>44767.490069444444</v>
+      </c>
+      <c r="G8" s="2">
+        <v>44779.515868055554</v>
+      </c>
+      <c r="H8" s="2"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="S8" s="1" t="s">
+        <v>78</v>
       </c>
       <c r="T8" s="1" t="s">
-        <v>50</v>
+        <v>74</v>
       </c>
       <c r="U8" s="1" t="s">
-        <v>64</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="V8" s="1"/>
+      <c r="W8" s="1"/>
+      <c r="X8" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="Y8" s="1"/>
       <c r="Z8" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="AA8" s="1" t="s">
         <v>44</v>
@@ -1445,8 +2428,9 @@
         <v>45</v>
       </c>
       <c r="AE8" s="1" t="s">
-        <v>53</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="AG8" s="1"/>
       <c r="AH8" s="1" t="s">
         <v>47</v>
       </c>
@@ -1468,34 +2452,49 @@
     </row>
     <row r="9" spans="1:39" ht="12.75">
       <c r="A9" s="1">
-        <v>19464</v>
+        <v>19454</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>65</v>
+        <v>39</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F9" s="3">
-        <v>44756.421030092592</v>
-      </c>
-      <c r="G9" s="3">
-        <v>44771.421030092592</v>
+        <v>192</v>
+      </c>
+      <c r="F9" s="2">
+        <v>44767.490069444444</v>
+      </c>
+      <c r="G9" s="2">
+        <v>44779.517500000002</v>
+      </c>
+      <c r="H9" s="2"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="S9" s="1" t="s">
+        <v>81</v>
       </c>
       <c r="T9" s="1" t="s">
-        <v>67</v>
+        <v>82</v>
       </c>
       <c r="U9" s="1" t="s">
-        <v>68</v>
-      </c>
+        <v>83</v>
+      </c>
+      <c r="V9" s="1"/>
+      <c r="W9" s="1"/>
+      <c r="X9" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="Y9" s="1"/>
       <c r="Z9" s="1" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="AA9" s="1" t="s">
         <v>44</v>
@@ -1510,8 +2509,9 @@
         <v>45</v>
       </c>
       <c r="AE9" s="1" t="s">
-        <v>53</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="AG9" s="1"/>
       <c r="AH9" s="1" t="s">
         <v>47</v>
       </c>
@@ -1533,34 +2533,50 @@
     </row>
     <row r="10" spans="1:39" ht="12.75">
       <c r="A10" s="1">
-        <v>19465</v>
+        <v>19455</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>69</v>
+        <v>39</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>70</v>
+        <v>85</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>70</v>
+        <v>85</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F10" s="3">
-        <v>44756.444884259261</v>
-      </c>
-      <c r="G10" s="3">
-        <v>44772.444884259261</v>
+        <v>192</v>
+      </c>
+      <c r="F10" s="2">
+        <v>44767.490069444444</v>
+      </c>
+      <c r="G10" s="2">
+        <v>44779.523275462961</v>
+      </c>
+      <c r="H10" s="2"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="S10" s="1" t="s">
+        <v>86</v>
       </c>
       <c r="T10" s="1" t="s">
-        <v>71</v>
+        <v>82</v>
       </c>
       <c r="U10" s="1" t="s">
-        <v>72</v>
-      </c>
+        <v>87</v>
+      </c>
+      <c r="V10" s="1"/>
+      <c r="W10" s="1"/>
+      <c r="X10" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="Y10" s="1"/>
       <c r="Z10" s="1" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="AA10" s="1" t="s">
         <v>44</v>
@@ -1575,8 +2591,9 @@
         <v>45</v>
       </c>
       <c r="AE10" s="1" t="s">
-        <v>53</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="AG10" s="1"/>
       <c r="AH10" s="1" t="s">
         <v>47</v>
       </c>
@@ -1598,34 +2615,50 @@
     </row>
     <row r="11" spans="1:39" ht="12.75">
       <c r="A11" s="1">
-        <v>19468</v>
+        <v>19456</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>73</v>
+        <v>39</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>74</v>
+        <v>89</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>74</v>
+        <v>89</v>
       </c>
       <c r="E11" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="F11" s="2">
+        <v>44767.490069444444</v>
+      </c>
+      <c r="G11" s="2">
+        <v>44779.530069444445</v>
+      </c>
+      <c r="H11" s="2"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="S11" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="T11" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F11" s="3">
-        <v>44756.506724537037</v>
-      </c>
-      <c r="G11" s="3">
-        <v>44779.506724537037</v>
-      </c>
-      <c r="T11" s="1" t="s">
-        <v>75</v>
-      </c>
       <c r="U11" s="1" t="s">
-        <v>76</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="V11" s="1"/>
+      <c r="W11" s="1"/>
+      <c r="X11" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="Y11" s="1"/>
       <c r="Z11" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="AA11" s="1" t="s">
         <v>44</v>
@@ -1640,8 +2673,9 @@
         <v>45</v>
       </c>
       <c r="AE11" s="1" t="s">
-        <v>53</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="AG11" s="1"/>
       <c r="AH11" s="1" t="s">
         <v>47</v>
       </c>
@@ -1663,34 +2697,50 @@
     </row>
     <row r="12" spans="1:39" ht="12.75">
       <c r="A12" s="1">
-        <v>19470</v>
+        <v>19468</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>77</v>
+        <v>92</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F12" s="3">
-        <v>44756.597604166665</v>
-      </c>
-      <c r="G12" s="3">
-        <v>44779.597604166665</v>
+        <v>192</v>
+      </c>
+      <c r="F12" s="2">
+        <v>44767.490069444444</v>
+      </c>
+      <c r="G12" s="2">
+        <v>44779.506724537037</v>
+      </c>
+      <c r="H12" s="2"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="S12" s="1" t="s">
+        <v>94</v>
       </c>
       <c r="T12" s="1" t="s">
-        <v>79</v>
+        <v>95</v>
       </c>
       <c r="U12" s="1" t="s">
-        <v>80</v>
-      </c>
+        <v>96</v>
+      </c>
+      <c r="V12" s="1"/>
+      <c r="W12" s="1"/>
+      <c r="X12" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="Y12" s="1"/>
       <c r="Z12" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="AA12" s="1" t="s">
         <v>44</v>
@@ -1705,8 +2755,9 @@
         <v>45</v>
       </c>
       <c r="AE12" s="1" t="s">
-        <v>53</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="AG12" s="1"/>
       <c r="AH12" s="1" t="s">
         <v>47</v>
       </c>
@@ -1728,34 +2779,50 @@
     </row>
     <row r="13" spans="1:39" ht="12.75">
       <c r="A13" s="1">
-        <v>19471</v>
+        <v>19470</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>81</v>
+        <v>98</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>82</v>
+        <v>99</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>82</v>
+        <v>99</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F13" s="3">
-        <v>44756.6950462963</v>
-      </c>
-      <c r="G13" s="3">
-        <v>44779.6950462963</v>
+        <v>192</v>
+      </c>
+      <c r="F13" s="2">
+        <v>44767.490069444444</v>
+      </c>
+      <c r="G13" s="2">
+        <v>44779.597604166665</v>
+      </c>
+      <c r="H13" s="2"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="S13" s="1" t="s">
+        <v>100</v>
       </c>
       <c r="T13" s="1" t="s">
-        <v>83</v>
+        <v>101</v>
       </c>
       <c r="U13" s="1" t="s">
-        <v>84</v>
-      </c>
+        <v>102</v>
+      </c>
+      <c r="V13" s="1"/>
+      <c r="W13" s="1"/>
+      <c r="X13" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="Y13" s="1"/>
       <c r="Z13" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="AA13" s="1" t="s">
         <v>44</v>
@@ -1770,8 +2837,9 @@
         <v>45</v>
       </c>
       <c r="AE13" s="1" t="s">
-        <v>53</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="AG13" s="1"/>
       <c r="AH13" s="1" t="s">
         <v>47</v>
       </c>
@@ -1793,34 +2861,50 @@
     </row>
     <row r="14" spans="1:39" ht="12.75">
       <c r="A14" s="1">
-        <v>19472</v>
+        <v>19471</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>85</v>
+        <v>104</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>86</v>
+        <v>105</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>86</v>
+        <v>105</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F14" s="3">
-        <v>44761.43645833333</v>
-      </c>
-      <c r="G14" s="3">
-        <v>44779.43645833333</v>
+        <v>192</v>
+      </c>
+      <c r="F14" s="2">
+        <v>44767.490069444444</v>
+      </c>
+      <c r="G14" s="2">
+        <v>44779.6950462963</v>
+      </c>
+      <c r="H14" s="2"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="S14" s="1" t="s">
+        <v>106</v>
       </c>
       <c r="T14" s="1" t="s">
-        <v>87</v>
+        <v>107</v>
       </c>
       <c r="U14" s="1" t="s">
-        <v>88</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="V14" s="1"/>
+      <c r="W14" s="1"/>
+      <c r="X14" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="Y14" s="1"/>
       <c r="Z14" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="AA14" s="1" t="s">
         <v>44</v>
@@ -1832,14 +2916,12 @@
         <v>44</v>
       </c>
       <c r="AD14" s="1" t="s">
-        <v>89</v>
+        <v>45</v>
       </c>
       <c r="AE14" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="AF14" s="2" t="s">
-        <v>91</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="AG14" s="1"/>
       <c r="AH14" s="1" t="s">
         <v>47</v>
       </c>
@@ -1861,34 +2943,49 @@
     </row>
     <row r="15" spans="1:39" ht="12.75">
       <c r="A15" s="1">
-        <v>19473</v>
+        <v>19472</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>85</v>
+        <v>110</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>92</v>
+        <v>111</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>92</v>
+        <v>111</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F15" s="3">
-        <v>44761.440983796296</v>
-      </c>
-      <c r="G15" s="3">
-        <v>44779.440983796296</v>
+        <v>192</v>
+      </c>
+      <c r="F15" s="2">
+        <v>44767.490069444444</v>
+      </c>
+      <c r="G15" s="2">
+        <v>44779.43645833333</v>
+      </c>
+      <c r="H15" s="2"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="S15" s="1" t="s">
+        <v>112</v>
       </c>
       <c r="T15" s="1" t="s">
-        <v>93</v>
+        <v>113</v>
       </c>
       <c r="U15" s="1" t="s">
-        <v>94</v>
-      </c>
+        <v>114</v>
+      </c>
+      <c r="V15" s="1"/>
+      <c r="W15" s="1"/>
+      <c r="X15" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="Y15" s="1"/>
       <c r="Z15" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="AA15" s="1" t="s">
         <v>44</v>
@@ -1900,14 +2997,15 @@
         <v>44</v>
       </c>
       <c r="AD15" s="1" t="s">
-        <v>89</v>
+        <v>116</v>
       </c>
       <c r="AE15" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="AF15" s="2" t="s">
-        <v>91</v>
-      </c>
+        <v>117</v>
+      </c>
+      <c r="AF15" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="AG15" s="1"/>
       <c r="AH15" s="1" t="s">
         <v>47</v>
       </c>
@@ -1932,31 +3030,42 @@
         <v>19474</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>85</v>
+        <v>110</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>95</v>
+        <v>119</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>95</v>
+        <v>119</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F16" s="3">
-        <v>44761.448634259257</v>
-      </c>
-      <c r="G16" s="3">
+        <v>192</v>
+      </c>
+      <c r="F16" s="2">
+        <v>44767.490069444444</v>
+      </c>
+      <c r="G16" s="2">
         <v>44779.448634259257</v>
       </c>
+      <c r="H16" s="2"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="2"/>
       <c r="T16" s="1" t="s">
-        <v>96</v>
+        <v>120</v>
       </c>
       <c r="U16" s="1" t="s">
-        <v>97</v>
-      </c>
+        <v>121</v>
+      </c>
+      <c r="V16" s="1"/>
+      <c r="W16" s="1"/>
+      <c r="X16" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="Y16" s="1"/>
       <c r="Z16" s="1" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="AA16" s="1" t="s">
         <v>44</v>
@@ -1968,14 +3077,15 @@
         <v>44</v>
       </c>
       <c r="AD16" s="1" t="s">
-        <v>89</v>
+        <v>116</v>
       </c>
       <c r="AE16" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="AF16" s="2" t="s">
-        <v>91</v>
-      </c>
+        <v>123</v>
+      </c>
+      <c r="AF16" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="AG16" s="1"/>
       <c r="AH16" s="1" t="s">
         <v>47</v>
       </c>
@@ -2000,31 +3110,47 @@
         <v>19475</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>99</v>
+        <v>124</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>99</v>
+        <v>124</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F17" s="3">
-        <v>44761.492465277777</v>
-      </c>
-      <c r="G17" s="3">
+        <v>192</v>
+      </c>
+      <c r="F17" s="2">
+        <v>44767.490069444444</v>
+      </c>
+      <c r="G17" s="2">
         <v>44779.492465277777</v>
       </c>
+      <c r="H17" s="2"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1"/>
+      <c r="S17" s="1" t="s">
+        <v>125</v>
+      </c>
       <c r="T17" s="1" t="s">
-        <v>100</v>
+        <v>126</v>
       </c>
       <c r="U17" s="1" t="s">
-        <v>101</v>
-      </c>
+        <v>127</v>
+      </c>
+      <c r="V17" s="1"/>
+      <c r="W17" s="1"/>
+      <c r="X17" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="Y17" s="1"/>
       <c r="Z17" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="AA17" s="1" t="s">
         <v>44</v>
@@ -2039,8 +3165,9 @@
         <v>45</v>
       </c>
       <c r="AE17" s="1" t="s">
-        <v>53</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="AG17" s="1"/>
       <c r="AH17" s="1" t="s">
         <v>47</v>
       </c>
@@ -2065,34 +3192,47 @@
         <v>19476</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>102</v>
+        <v>129</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>103</v>
+        <v>130</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>103</v>
+        <v>130</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F18" s="3">
-        <v>44761.546574074076</v>
-      </c>
-      <c r="G18" s="3">
+        <v>192</v>
+      </c>
+      <c r="F18" s="2">
+        <v>44767.490069444444</v>
+      </c>
+      <c r="G18" s="2">
         <v>44779.546574074076</v>
       </c>
+      <c r="H18" s="2"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="1"/>
+      <c r="N18" s="1"/>
+      <c r="S18" s="1" t="s">
+        <v>131</v>
+      </c>
       <c r="T18" s="1" t="s">
-        <v>104</v>
+        <v>132</v>
       </c>
       <c r="U18" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="X18" s="2" t="s">
-        <v>106</v>
-      </c>
+        <v>133</v>
+      </c>
+      <c r="V18" s="1"/>
+      <c r="W18" s="1"/>
+      <c r="X18" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="Y18" s="1"/>
       <c r="Z18" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="AA18" s="1" t="s">
         <v>44</v>
@@ -2107,8 +3247,9 @@
         <v>45</v>
       </c>
       <c r="AE18" s="1" t="s">
-        <v>53</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="AG18" s="1"/>
       <c r="AH18" s="1" t="s">
         <v>47</v>
       </c>
@@ -2133,31 +3274,47 @@
         <v>19477</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>65</v>
+        <v>135</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>107</v>
+        <v>136</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>107</v>
+        <v>136</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F19" s="3">
-        <v>44761.597731481481</v>
-      </c>
-      <c r="G19" s="3">
+        <v>192</v>
+      </c>
+      <c r="F19" s="2">
+        <v>44767.490069444444</v>
+      </c>
+      <c r="G19" s="2">
         <v>44779.597731481481</v>
       </c>
+      <c r="H19" s="2"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="2"/>
+      <c r="M19" s="1"/>
+      <c r="N19" s="1"/>
+      <c r="S19" s="1" t="s">
+        <v>137</v>
+      </c>
       <c r="T19" s="1" t="s">
-        <v>108</v>
+        <v>138</v>
       </c>
       <c r="U19" s="1" t="s">
-        <v>109</v>
-      </c>
+        <v>139</v>
+      </c>
+      <c r="V19" s="1"/>
+      <c r="W19" s="1"/>
+      <c r="X19" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="Y19" s="1"/>
       <c r="Z19" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="AA19" s="1" t="s">
         <v>44</v>
@@ -2172,8 +3329,9 @@
         <v>45</v>
       </c>
       <c r="AE19" s="1" t="s">
-        <v>53</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="AG19" s="1"/>
       <c r="AH19" s="1" t="s">
         <v>47</v>
       </c>
@@ -2198,34 +3356,47 @@
         <v>19478</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>110</v>
+        <v>141</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>111</v>
+        <v>142</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>111</v>
+        <v>142</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F20" s="3">
-        <v>44761.676701388889</v>
-      </c>
-      <c r="G20" s="3">
+        <v>192</v>
+      </c>
+      <c r="F20" s="2">
+        <v>44767.490069444444</v>
+      </c>
+      <c r="G20" s="2">
         <v>44779.676701388889</v>
       </c>
+      <c r="H20" s="2"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="2"/>
+      <c r="M20" s="1"/>
+      <c r="N20" s="1"/>
+      <c r="S20" s="1" t="s">
+        <v>143</v>
+      </c>
       <c r="T20" s="1" t="s">
-        <v>112</v>
+        <v>144</v>
       </c>
       <c r="U20" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="X20" s="2" t="s">
-        <v>114</v>
-      </c>
+        <v>145</v>
+      </c>
+      <c r="V20" s="1"/>
+      <c r="W20" s="1"/>
+      <c r="X20" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="Y20" s="1"/>
       <c r="Z20" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="AA20" s="1" t="s">
         <v>44</v>
@@ -2240,8 +3411,9 @@
         <v>45</v>
       </c>
       <c r="AE20" s="1" t="s">
-        <v>115</v>
-      </c>
+        <v>147</v>
+      </c>
+      <c r="AG20" s="1"/>
       <c r="AH20" s="1" t="s">
         <v>47</v>
       </c>
@@ -2260,8 +3432,582 @@
       <c r="AM20" s="1" t="s">
         <v>44</v>
       </c>
+    </row>
+    <row r="21" spans="1:39" ht="12.75">
+      <c r="A21" s="1">
+        <v>19479</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="F21" s="2">
+        <v>44767.490069444444</v>
+      </c>
+      <c r="G21" s="2">
+        <v>44772.505162037036</v>
+      </c>
+      <c r="H21" s="2"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+      <c r="M21" s="1"/>
+      <c r="N21" s="1"/>
+      <c r="S21" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="T21" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="U21" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="V21" s="1"/>
+      <c r="W21" s="1"/>
+      <c r="X21" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="Y21" s="1"/>
+      <c r="Z21" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA21" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB21" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC21" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AD21" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="AE21" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="AF21" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="AG21" s="1"/>
+      <c r="AH21" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AI21" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AJ21" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AK21" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AL21" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AM21" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="1:39" ht="12.75">
+      <c r="A22" s="1">
+        <v>19481</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="F22" s="2">
+        <v>44767.490069444444</v>
+      </c>
+      <c r="G22" s="2">
+        <v>44772.545972222222</v>
+      </c>
+      <c r="H22" s="2"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="2"/>
+      <c r="M22" s="1"/>
+      <c r="N22" s="1"/>
+      <c r="S22" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="T22" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="U22" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="V22" s="1"/>
+      <c r="W22" s="1"/>
+      <c r="X22" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="Y22" s="1"/>
+      <c r="Z22" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA22" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB22" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC22" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AD22" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AE22" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AG22" s="1"/>
+      <c r="AH22" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AI22" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AJ22" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AK22" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AL22" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AM22" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="1:39" ht="12.75">
+      <c r="A23" s="1">
+        <v>19482</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="F23" s="2">
+        <v>44767.490069444444</v>
+      </c>
+      <c r="G23" s="2">
+        <v>44779.584641203706</v>
+      </c>
+      <c r="H23" s="2"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+      <c r="M23" s="1"/>
+      <c r="N23" s="1"/>
+      <c r="S23" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="T23" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="U23" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="V23" s="1"/>
+      <c r="W23" s="1"/>
+      <c r="X23" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="Y23" s="1"/>
+      <c r="Z23" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA23" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB23" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC23" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AD23" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AE23" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="AG23" s="1"/>
+      <c r="AH23" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AI23" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AJ23" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AK23" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AL23" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AM23" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" spans="1:39" ht="12.75">
+      <c r="A24" s="1">
+        <v>19483</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="F24" s="2">
+        <v>44767.490069444444</v>
+      </c>
+      <c r="G24" s="2">
+        <v>44779.693981481483</v>
+      </c>
+      <c r="H24" s="2"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+      <c r="M24" s="1"/>
+      <c r="N24" s="1"/>
+      <c r="S24" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="T24" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="U24" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="V24" s="1"/>
+      <c r="W24" s="1"/>
+      <c r="X24" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="Y24" s="1"/>
+      <c r="Z24" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA24" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB24" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC24" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AD24" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AE24" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AG24" s="1"/>
+      <c r="AH24" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AI24" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AJ24" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AK24" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AL24" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AM24" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" spans="1:39" ht="12.75">
+      <c r="A25" s="1">
+        <v>19484</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="F25" s="2">
+        <v>44767.490069444444</v>
+      </c>
+      <c r="G25" s="2">
+        <v>44779.411574074074</v>
+      </c>
+      <c r="H25" s="2"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+      <c r="K25" s="1"/>
+      <c r="M25" s="1"/>
+      <c r="N25" s="1"/>
+      <c r="S25" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="T25" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="U25" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="V25" s="1"/>
+      <c r="W25" s="1"/>
+      <c r="Y25" s="1"/>
+      <c r="Z25" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA25" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB25" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC25" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AD25" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AE25" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AG25" s="1"/>
+      <c r="AH25" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AI25" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AJ25" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AK25" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AL25" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AM25" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="26" spans="1:39" ht="12.75">
+      <c r="A26" s="1">
+        <v>19492</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="F26" s="2">
+        <v>44767.490069444444</v>
+      </c>
+      <c r="G26" s="2">
+        <v>44779.482685185183</v>
+      </c>
+      <c r="H26" s="2"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+      <c r="K26" s="1"/>
+      <c r="L26" s="2"/>
+      <c r="M26" s="1"/>
+      <c r="N26" s="1"/>
+      <c r="S26" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="T26" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="U26" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="V26" s="1"/>
+      <c r="W26" s="1"/>
+      <c r="X26" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="Y26" s="1"/>
+      <c r="Z26" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA26" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB26" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC26" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AD26" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AG26" s="1"/>
+      <c r="AH26" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AI26" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AJ26" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AK26" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AL26" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AM26" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="27" spans="1:39" ht="12.75">
+      <c r="A27" s="1">
+        <v>19497</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="F27" s="2">
+        <v>44767.490069444444</v>
+      </c>
+      <c r="G27" s="2">
+        <v>44772.566944444443</v>
+      </c>
+      <c r="H27" s="2"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+      <c r="K27" s="1"/>
+      <c r="L27" s="2"/>
+      <c r="M27" s="1"/>
+      <c r="N27" s="1"/>
+      <c r="S27" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="T27" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="U27" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="V27" s="1"/>
+      <c r="W27" s="1"/>
+      <c r="X27" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="Y27" s="1"/>
+      <c r="Z27" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA27" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB27" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC27" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AD27" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="AE27" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="AF27" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="AG27" s="1"/>
+      <c r="AH27" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AI27" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AJ27" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AK27" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AL27" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AM27" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="31" spans="6:6" ht="12.75">
+      <c r="F31" s="2"/>
     </row>
   </sheetData>
+  <sheetProtection/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter alignWithMargins="0">
     <oddHeader>&amp;C&amp;A</oddHeader>
@@ -2271,7 +4017,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{bfabce41-31b7-452f-9fe7-44315e96c41a}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2e95c94e-23f4-4c96-93b6-055fbbc84dc5}">
   <dimension ref="A5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A1"/>
@@ -2279,8 +4025,8 @@
   <sheetFormatPr defaultRowHeight="12.75"/>
   <sheetData>
     <row r="5" spans="1:1" ht="23.25" customHeight="1">
-      <c r="A5" s="4" t="s">
-        <v>116</v>
+      <c r="A5" s="3" t="s">
+        <v>193</v>
       </c>
     </row>
   </sheetData>

</xml_diff>